<commit_message>
Normalize columns to build python identifiers
</commit_message>
<xml_diff>
--- a/tests/test.xlsx
+++ b/tests/test.xlsx
@@ -24,7 +24,7 @@
     <t>Foo</t>
   </si>
   <si>
-    <t>Bar</t>
+    <t>Bar/Bu</t>
   </si>
 </sst>
 </file>
@@ -396,7 +396,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>